<commit_message>
Last updates on the file and creating a copy in PDF format
</commit_message>
<xml_diff>
--- a/docs/product_backlog.xlsx
+++ b/docs/product_backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santo\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mirax\No_backup\ing\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF2367C-30D7-4E83-A7F0-61CDB8B47A4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C8AA65-3F50-4B06-9F9E-636840134442}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -19,48 +19,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Esempio:
-"The user may consult the system to make wine inventory, i.e. check which wines are in inventory"
-	-Luca Santoro</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>"The &lt;&lt;How to demonstrate&gt;&gt; field of the implemented user stories should be linked to the documentation of the service which implements it"
-	-Luca Santoro
-Esempio:
-• A table with all wines and their property is visualized
-• &lt;eccezioni&gt;
-• link to the page of the feature
-	-Luca Santoro</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
   <si>
@@ -104,9 +62,6 @@
   </si>
   <si>
     <t>Ottieni film tramite un codice identificativo</t>
-  </si>
-  <si>
-    <t>Possibilità di visualizzare il film che corrisponde all'id</t>
   </si>
   <si>
     <t>Aprire la pagina al PATH definito, verrà ritornato il film presente nel sistema in base all'ID specificato</t>
@@ -145,9 +100,6 @@
     <t>Inserisci un nuovo film</t>
   </si>
   <si>
-    <t>Solo tramite autenticazione, possibilità di inserire un nuovo film</t>
-  </si>
-  <si>
     <t>Aprire la pagina al PATH definito, autenticarsi, e successivamente inviare le informazioni relative al film da inserire</t>
   </si>
   <si>
@@ -161,9 +113,6 @@
   </si>
   <si>
     <t>Ottieni un film tramite il suo titolo</t>
-  </si>
-  <si>
-    <t>Possibilità di visualizzare tutti i film che corrispondono al titolo del film che sto cercando</t>
   </si>
   <si>
     <t>Aprire la pagina al PATH definito, verranno ritornati tutti i film presenti nel sistema in base al titolo specificato</t>
@@ -193,9 +142,6 @@
     <t>Cancella un film tramite il codice identificativo</t>
   </si>
   <si>
-    <t>Solo tramite autenticazione, possibilità di rimuovere un film</t>
-  </si>
-  <si>
     <t>Aprire la pagina al PATH definito, autenticarsi, e successivamente definire il film da eliminare dal sistema</t>
   </si>
   <si>
@@ -205,55 +151,67 @@
     <t>Ottieni un film in base al genere</t>
   </si>
   <si>
-    <t>Possibilità di visualizzare tutti i film in base al genere</t>
-  </si>
-  <si>
     <t>Aprire la pagina al PATH definito, verranno ritornati tutti i film presenti nel sistema in base al genere specificato</t>
   </si>
   <si>
     <t>Ottieni un film in base all'anno di produzione</t>
   </si>
   <si>
-    <t>Possibilità di visualizzare tutti i film di un particolare anno</t>
-  </si>
-  <si>
     <t>Aprire la pagina al PATH definito, verranno ritornati tutti i film presenti nel sistema in base all'anno specificato</t>
   </si>
   <si>
     <t>Ottieni un film in base al nome o identificativo di un attore</t>
   </si>
   <si>
-    <t>Possibilità di visualizzare tutti i film dove ha collaborato un determinato attore</t>
-  </si>
-  <si>
     <t>Aprire la pagina al PATH definito, verranno ritornati tutti i film presenti nel sistema in base all'attore spedificato</t>
   </si>
   <si>
     <t>Ottieni un film tramite il nome o identificativo del/dei regista</t>
   </si>
   <si>
-    <t>Possibilità di visualizzare tutti i film dove ha collaborato un determinato regista</t>
-  </si>
-  <si>
     <t>Aprire la pagina al PATH definito, verranno ritornati tutti i film presenti nel sistema in base al regista specificato</t>
   </si>
   <si>
     <t>Modificare i dati di un film</t>
   </si>
   <si>
-    <t>Solo tramite autenticazione, possibilità di modificare un film</t>
-  </si>
-  <si>
     <t>Aprire la pagina al PATH definito, autenticarsi, e successivamente definire il film con le relative informazioni da modificare</t>
   </si>
   <si>
     <t>Ottienere tutti i film presenti nel sistema</t>
   </si>
   <si>
-    <t>Possibilità di visualizzare tutti i film presenti nel sistema</t>
-  </si>
-  <si>
     <t>Aprire la pagina al PATH definito, verrà ritornata la lista di tutti i film presenti nel sistema</t>
+  </si>
+  <si>
+    <t>L'amministratore vuole inserire un film nel catolgo</t>
+  </si>
+  <si>
+    <t>L'utente vuole vedere le informazioni relative ad un film digitando il suo titolo</t>
+  </si>
+  <si>
+    <t>L'amministratore vuole elimiare un film dal catolgo</t>
+  </si>
+  <si>
+    <t>L'utente vuole vedere le informazioni relative ai film in base al genere</t>
+  </si>
+  <si>
+    <t>L'utente vuole vedere le informazioni relative ai film in base all'anno di produzione</t>
+  </si>
+  <si>
+    <t>L'utente vuole vedere le informazioni relative ai film in base ad un determinato attore</t>
+  </si>
+  <si>
+    <t>L'utente vuole vedere le informazioni relative ai film in base ad un determinato regista</t>
+  </si>
+  <si>
+    <t>L'amministratore vuole modificare un film dal catolgo</t>
+  </si>
+  <si>
+    <t>L'utente vuole un determinato film in base al suo codice identificativo</t>
+  </si>
+  <si>
+    <t>L'utente vuole vedere tutti i film presenti nel catalogo</t>
   </si>
 </sst>
 </file>
@@ -1015,14 +973,20 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1031,18 +995,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -1279,32 +1237,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:AA19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="50" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="5.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="6" max="7" width="21.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" customWidth="1"/>
-    <col min="15" max="15" width="21.42578125" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="5.86328125" customWidth="1"/>
+    <col min="3" max="3" width="19.3984375" customWidth="1"/>
+    <col min="4" max="4" width="15.3984375" customWidth="1"/>
+    <col min="6" max="7" width="21.73046875" customWidth="1"/>
+    <col min="8" max="8" width="18.265625" customWidth="1"/>
+    <col min="10" max="10" width="5.86328125" customWidth="1"/>
+    <col min="11" max="11" width="15.86328125" customWidth="1"/>
+    <col min="14" max="14" width="20.86328125" customWidth="1"/>
+    <col min="15" max="15" width="21.3984375" customWidth="1"/>
+    <col min="16" max="16" width="17.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="64" t="s">
+    <row r="2" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="73" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="65"/>
@@ -1314,7 +1273,7 @@
       <c r="G2" s="65"/>
       <c r="H2" s="66"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="70" t="s">
+      <c r="J2" s="74" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="65"/>
@@ -1323,53 +1282,53 @@
       <c r="N2" s="65"/>
       <c r="O2" s="65"/>
       <c r="P2" s="66"/>
-      <c r="R2" s="71" t="s">
+      <c r="R2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="74" t="s">
+      <c r="S2" s="64" t="s">
         <v>3</v>
       </c>
       <c r="T2" s="65"/>
-      <c r="U2" s="75"/>
-      <c r="V2" s="74" t="s">
+      <c r="U2" s="78"/>
+      <c r="V2" s="64" t="s">
         <v>4</v>
       </c>
       <c r="W2" s="65"/>
       <c r="X2" s="66"/>
-      <c r="Y2" s="74" t="s">
+      <c r="Y2" s="64" t="s">
         <v>5</v>
       </c>
       <c r="Z2" s="65"/>
       <c r="AA2" s="66"/>
     </row>
-    <row r="3" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="67"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="69"/>
+    <row r="3" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="70"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="72"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="68"/>
-      <c r="N3" s="68"/>
-      <c r="O3" s="68"/>
-      <c r="P3" s="69"/>
-      <c r="R3" s="72"/>
-      <c r="S3" s="76"/>
-      <c r="T3" s="77"/>
-      <c r="U3" s="78"/>
-      <c r="V3" s="76"/>
-      <c r="W3" s="77"/>
-      <c r="X3" s="80"/>
-      <c r="Y3" s="76"/>
-      <c r="Z3" s="77"/>
-      <c r="AA3" s="80"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="71"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="72"/>
+      <c r="R3" s="76"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="79"/>
+      <c r="V3" s="67"/>
+      <c r="W3" s="68"/>
+      <c r="X3" s="69"/>
+      <c r="Y3" s="67"/>
+      <c r="Z3" s="68"/>
+      <c r="AA3" s="69"/>
     </row>
-    <row r="4" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1413,18 +1372,18 @@
       <c r="P4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="73"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="68"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="67"/>
-      <c r="W4" s="68"/>
-      <c r="X4" s="69"/>
-      <c r="Y4" s="67"/>
-      <c r="Z4" s="68"/>
-      <c r="AA4" s="69"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="70"/>
+      <c r="T4" s="71"/>
+      <c r="U4" s="80"/>
+      <c r="V4" s="70"/>
+      <c r="W4" s="71"/>
+      <c r="X4" s="72"/>
+      <c r="Y4" s="70"/>
+      <c r="Z4" s="71"/>
+      <c r="AA4" s="72"/>
     </row>
-    <row r="5" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="11">
         <v>1</v>
       </c>
@@ -1438,13 +1397,13 @@
         <v>5</v>
       </c>
       <c r="F5" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="H5" s="14" t="s">
         <v>15</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>16</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="15">
@@ -1459,26 +1418,26 @@
       <c r="M5" s="17">
         <v>5</v>
       </c>
-      <c r="N5" s="17" t="s">
+      <c r="N5" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="O5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="17" t="s">
+      <c r="P5" s="18" t="s">
         <v>15</v>
-      </c>
-      <c r="P5" s="18" t="s">
-        <v>16</v>
       </c>
       <c r="R5" s="19">
         <v>1</v>
       </c>
       <c r="S5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="T5" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="T5" s="21" t="s">
+      <c r="U5" s="22" t="s">
         <v>18</v>
-      </c>
-      <c r="U5" s="22" t="s">
-        <v>19</v>
       </c>
       <c r="V5" s="23"/>
       <c r="W5" s="24"/>
@@ -1487,12 +1446,12 @@
       <c r="Z5" s="26"/>
       <c r="AA5" s="27"/>
     </row>
-    <row r="6" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="28">
         <v>2</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="30">
         <v>100</v>
@@ -1501,20 +1460,20 @@
         <v>8</v>
       </c>
       <c r="F6" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="31" t="s">
         <v>21</v>
-      </c>
-      <c r="G6" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="31" t="s">
-        <v>23</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="32">
         <v>2</v>
       </c>
       <c r="K6" s="29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L6" s="33">
         <v>100</v>
@@ -1522,26 +1481,26 @@
       <c r="M6" s="34">
         <v>8</v>
       </c>
-      <c r="N6" s="34" t="s">
+      <c r="N6" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="O6" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="P6" s="35" t="s">
         <v>21</v>
-      </c>
-      <c r="O6" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="P6" s="35" t="s">
-        <v>23</v>
       </c>
       <c r="R6" s="36">
         <v>2</v>
       </c>
       <c r="S6" s="37" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="T6" s="38" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="U6" s="39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="V6" s="40"/>
       <c r="W6" s="41"/>
@@ -1550,12 +1509,12 @@
       <c r="Z6" s="41"/>
       <c r="AA6" s="43"/>
     </row>
-    <row r="7" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="28">
         <v>3</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" s="30">
         <v>90</v>
@@ -1564,20 +1523,20 @@
         <v>7</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="44">
         <v>3</v>
       </c>
       <c r="K7" s="45" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L7" s="46">
         <v>90</v>
@@ -1585,26 +1544,26 @@
       <c r="M7" s="47">
         <v>7</v>
       </c>
-      <c r="N7" s="47" t="s">
-        <v>27</v>
+      <c r="N7" s="30" t="s">
+        <v>43</v>
       </c>
       <c r="O7" s="47" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="P7" s="48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R7" s="49">
         <v>3</v>
       </c>
       <c r="S7" s="50" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="T7" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="U7" s="52" t="s">
         <v>18</v>
-      </c>
-      <c r="U7" s="52" t="s">
-        <v>19</v>
       </c>
       <c r="V7" s="53"/>
       <c r="W7" s="53"/>
@@ -1613,12 +1572,12 @@
       <c r="Z7" s="55"/>
       <c r="AA7" s="56"/>
     </row>
-    <row r="8" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="28">
         <v>4</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D8" s="30">
         <v>85</v>
@@ -1627,13 +1586,13 @@
         <v>3</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="57"/>
@@ -1644,16 +1603,16 @@
       <c r="O8" s="58"/>
       <c r="P8" s="58"/>
       <c r="V8" s="59" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="X8" s="59"/>
     </row>
-    <row r="9" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="28">
         <v>5</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D9" s="30">
         <v>50</v>
@@ -1662,13 +1621,13 @@
         <v>7</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="G9" s="30" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H9" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1677,12 +1636,12 @@
       <c r="M9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="28">
         <v>6</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D10" s="30">
         <v>40</v>
@@ -1691,13 +1650,13 @@
         <v>4</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="G10" s="30" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H10" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1707,12 +1666,12 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="28">
         <v>7</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D11" s="30">
         <v>20</v>
@@ -1721,13 +1680,13 @@
         <v>7</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1738,12 +1697,12 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="28">
         <v>8</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D12" s="30">
         <v>20</v>
@@ -1752,13 +1711,13 @@
         <v>7</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H12" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1769,12 +1728,12 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="28">
         <v>9</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D13" s="30">
         <v>15</v>
@@ -1783,13 +1742,13 @@
         <v>6</v>
       </c>
       <c r="F13" s="30" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1800,12 +1759,12 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:27" ht="114" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="60">
         <v>10</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D14" s="46">
         <v>10</v>
@@ -1814,13 +1773,13 @@
         <v>5</v>
       </c>
       <c r="F14" s="46" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G14" s="46" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="H14" s="61" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1831,25 +1790,25 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:27" ht="12.75" x14ac:dyDescent="0.35">
       <c r="D15" s="62"/>
     </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:27" ht="12.75" x14ac:dyDescent="0.35">
       <c r="D16" s="62"/>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="D17" s="62"/>
       <c r="F17" s="63"/>
       <c r="G17" s="63"/>
       <c r="H17" s="63"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="D18" s="62"/>
       <c r="F18" s="63"/>
       <c r="G18" s="63"/>
       <c r="H18" s="63"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:8" ht="12.75" x14ac:dyDescent="0.35">
       <c r="D19" s="62"/>
       <c r="F19" s="63"/>
       <c r="G19" s="63"/>
@@ -1883,6 +1842,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" scale="32" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>